<commit_message>
add antibody related fields
</commit_message>
<xml_diff>
--- a/sequencing_spreadsheet.template.xlsx
+++ b/sequencing_spreadsheet.template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="231">
   <si>
     <t xml:space="preserve">SORTING</t>
   </si>
@@ -167,6 +167,15 @@
   </si>
   <si>
     <t xml:space="preserve">LANES_TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANTIBODY_TARGET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANTIBODY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANTIBODY_LOT</t>
   </si>
   <si>
     <t xml:space="preserve">NOTES</t>
@@ -1281,11 +1290,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE13" activeCellId="0" sqref="AE13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AQ1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AZ2" activeCellId="0" sqref="AZ2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.37"/>
@@ -1316,11 +1325,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="39.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="30.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="20.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="50.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="51" style="1" width="20.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="1" width="18.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="1" width="33.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="62" style="1" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="50" style="1" width="50.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="54" style="1" width="20.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="1" width="18.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="1" width="33.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="65" style="1" width="10.99"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="66.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1501,23 +1510,32 @@
       <c r="BG1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="8" t="s">
+      <c r="BH1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="8" t="s">
+      <c r="BI1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="8"/>
+      <c r="BJ1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="8"/>
     </row>
     <row r="2" s="14" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="12"/>
@@ -1528,77 +1546,77 @@
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="X2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="Y2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="Z2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AB2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AD2" s="12"/>
       <c r="AE2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AF2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AG2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AH2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AI2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AJ2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AK2" s="12"/>
       <c r="AL2" s="12"/>
@@ -1610,19 +1628,19 @@
       <c r="AR2" s="12"/>
       <c r="AS2" s="12"/>
       <c r="AT2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AU2" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AV2" s="12"/>
       <c r="AW2" s="12"/>
-      <c r="AX2" s="12" t="s">
-        <v>64</v>
-      </c>
+      <c r="AX2" s="12"/>
       <c r="AY2" s="12"/>
       <c r="AZ2" s="12"/>
-      <c r="BA2" s="12"/>
+      <c r="BA2" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="BB2" s="12"/>
       <c r="BC2" s="12"/>
       <c r="BD2" s="12"/>
@@ -1632,10 +1650,10 @@
       <c r="BH2" s="12"/>
       <c r="BI2" s="12"/>
       <c r="BJ2" s="12"/>
-      <c r="BK2" s="13"/>
-      <c r="AMA2" s="13"/>
-      <c r="AMB2" s="13"/>
-      <c r="AMC2" s="13"/>
+      <c r="BK2" s="12"/>
+      <c r="BL2" s="12"/>
+      <c r="BM2" s="12"/>
+      <c r="BN2" s="13"/>
       <c r="AMD2" s="13"/>
       <c r="AME2" s="13"/>
       <c r="AMF2" s="13"/>
@@ -1646,16 +1664,16 @@
     </row>
     <row r="3" s="20" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>62</v>
-      </c>
       <c r="C3" s="16" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E3" s="17"/>
       <c r="F3" s="18" t="s">
@@ -1665,16 +1683,16 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="18" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="M3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="N3" s="19"/>
       <c r="O3" s="19"/>
@@ -1682,66 +1700,66 @@
       <c r="Q3" s="19"/>
       <c r="R3" s="19"/>
       <c r="S3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="T3" s="19"/>
       <c r="U3" s="19"/>
       <c r="V3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="W3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="X3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="Y3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="Z3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AA3" s="19"/>
       <c r="AB3" s="19"/>
       <c r="AC3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AD3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AE3" s="19" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="AF3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AG3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AH3" s="19"/>
       <c r="AI3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AJ3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AK3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AL3" s="19"/>
       <c r="AM3" s="19"/>
       <c r="AN3" s="19"/>
       <c r="AO3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AP3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AQ3" s="19"/>
       <c r="AR3" s="19"/>
       <c r="AS3" s="19"/>
       <c r="AT3" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AU3" s="19"/>
       <c r="AV3" s="19"/>
@@ -1759,131 +1777,131 @@
       <c r="BH3" s="19"/>
       <c r="BI3" s="19"/>
       <c r="BJ3" s="19"/>
+      <c r="BK3" s="19"/>
+      <c r="BL3" s="19"/>
+      <c r="BM3" s="19"/>
     </row>
     <row r="4" s="22" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="21" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L4" s="22" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M4" s="22" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="N4" s="22" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="R4" s="23" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="S4" s="22" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="T4" s="23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U4" s="22" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="V4" s="22" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="W4" s="22" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="X4" s="22" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="Y4" s="22" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="Z4" s="22" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AA4" s="22" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="AB4" s="22" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="AC4" s="24" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AD4" s="25"/>
       <c r="AE4" s="26"/>
       <c r="AF4" s="25"/>
       <c r="AG4" s="27"/>
       <c r="AH4" s="22" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="AL4" s="22" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="AO4" s="22" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AP4" s="22" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AQ4" s="22" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="AT4" s="22" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="AU4" s="22" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="AV4" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="AX4" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="BE4" s="27"/>
-      <c r="BF4" s="27"/>
-      <c r="BG4" s="28"/>
-      <c r="BH4" s="28" t="n">
+        <v>104</v>
+      </c>
+      <c r="BA4" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="BH4" s="27"/>
+      <c r="BI4" s="27"/>
+      <c r="BJ4" s="28"/>
+      <c r="BK4" s="28" t="n">
         <v>123456</v>
       </c>
-      <c r="BI4" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="BJ4" s="28"/>
-      <c r="BK4" s="28"/>
-      <c r="AMA4" s="28"/>
-      <c r="AMB4" s="28"/>
-      <c r="AMC4" s="28"/>
+      <c r="BL4" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="BM4" s="28"/>
+      <c r="BN4" s="28"/>
       <c r="AMD4" s="28"/>
       <c r="AME4" s="28"/>
       <c r="AMF4" s="28"/>
@@ -1894,115 +1912,112 @@
     </row>
     <row r="5" s="22" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="21" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="L5" s="29" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="M5" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="R5" s="23"/>
       <c r="S5" s="23" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="T5" s="23"/>
       <c r="U5" s="22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="V5" s="22" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="Y5" s="22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="Z5" s="22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AA5" s="22" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="AB5" s="30" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AC5" s="31"/>
       <c r="AD5" s="25"/>
       <c r="AE5" s="26" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AF5" s="25" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AG5" s="27" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AH5" s="22" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="AI5" s="22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="AJ5" s="22" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="AK5" s="22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="AL5" s="22" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="AQ5" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="AU5" s="22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AV5" s="23"/>
-      <c r="AX5" s="23"/>
-      <c r="BE5" s="27"/>
-      <c r="BF5" s="27"/>
-      <c r="BG5" s="28"/>
-      <c r="BH5" s="28" t="n">
+      <c r="BA5" s="23"/>
+      <c r="BH5" s="27"/>
+      <c r="BI5" s="27"/>
+      <c r="BJ5" s="28"/>
+      <c r="BK5" s="28" t="n">
         <v>123456</v>
       </c>
-      <c r="BI5" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="BJ5" s="28"/>
-      <c r="BK5" s="28"/>
-      <c r="AMA5" s="28"/>
-      <c r="AMB5" s="28"/>
-      <c r="AMC5" s="28"/>
+      <c r="BL5" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="BM5" s="28"/>
+      <c r="BN5" s="28"/>
       <c r="AMD5" s="28"/>
       <c r="AME5" s="28"/>
       <c r="AMF5" s="28"/>
@@ -2011,39 +2026,39 @@
       <c r="AMI5" s="28"/>
       <c r="AMJ5" s="28"/>
     </row>
-    <row r="6" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="21" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="L6" s="29" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="N6" s="28"/>
       <c r="O6" s="28"/>
@@ -2051,64 +2066,61 @@
       <c r="Q6" s="28"/>
       <c r="R6" s="23"/>
       <c r="S6" s="23" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="T6" s="23"/>
       <c r="U6" s="22" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="V6" s="22" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="Y6" s="22" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="Z6" s="22" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="AA6" s="22" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AB6" s="22" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AC6" s="31"/>
       <c r="AD6" s="25"/>
       <c r="AE6" s="22" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="AF6" s="25"/>
       <c r="AG6" s="27"/>
       <c r="AH6" s="22" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="AI6" s="27" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="AJ6" s="22" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AK6" s="22" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="AL6" s="22" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="AU6" s="14" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="AV6" s="23"/>
-      <c r="AX6" s="23"/>
-      <c r="BE6" s="27"/>
-      <c r="BF6" s="27"/>
-      <c r="BG6" s="28"/>
-      <c r="BH6" s="28"/>
-      <c r="BI6" s="28"/>
+      <c r="BA6" s="23"/>
+      <c r="BH6" s="27"/>
+      <c r="BI6" s="27"/>
       <c r="BJ6" s="28"/>
       <c r="BK6" s="28"/>
-      <c r="AMA6" s="28"/>
-      <c r="AMB6" s="28"/>
-      <c r="AMC6" s="28"/>
+      <c r="BL6" s="28"/>
+      <c r="BM6" s="28"/>
+      <c r="BN6" s="28"/>
       <c r="AMD6" s="28"/>
       <c r="AME6" s="28"/>
       <c r="AMF6" s="28"/>
@@ -2117,36 +2129,36 @@
       <c r="AMI6" s="28"/>
       <c r="AMJ6" s="28"/>
     </row>
-    <row r="7" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="32" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="N7" s="22" t="n">
         <v>1</v>
@@ -2155,64 +2167,61 @@
         <v>1</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="Q7" s="22" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="R7" s="23"/>
       <c r="S7" s="23" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="T7" s="22" t="n">
         <v>924</v>
       </c>
       <c r="U7" s="22" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="W7" s="22" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="X7" s="22" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="AA7" s="22" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="AB7" s="28"/>
       <c r="AC7" s="26"/>
       <c r="AD7" s="25"/>
       <c r="AE7" s="33" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="AF7" s="25"/>
       <c r="AG7" s="27"/>
       <c r="AH7" s="22" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="AI7" s="22" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="AL7" s="22" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="AT7" s="22" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="AU7" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="AX7" s="23"/>
-      <c r="BE7" s="27"/>
-      <c r="BF7" s="27"/>
-      <c r="BG7" s="28"/>
-      <c r="BH7" s="28"/>
-      <c r="BI7" s="28"/>
+        <v>175</v>
+      </c>
+      <c r="BA7" s="23"/>
+      <c r="BH7" s="27"/>
+      <c r="BI7" s="27"/>
       <c r="BJ7" s="28"/>
       <c r="BK7" s="28"/>
-      <c r="AMA7" s="28"/>
-      <c r="AMB7" s="28"/>
-      <c r="AMC7" s="28"/>
+      <c r="BL7" s="28"/>
+      <c r="BM7" s="28"/>
+      <c r="BN7" s="28"/>
       <c r="AMD7" s="28"/>
       <c r="AME7" s="28"/>
       <c r="AMF7" s="28"/>
@@ -2221,91 +2230,88 @@
       <c r="AMI7" s="28"/>
       <c r="AMJ7" s="28"/>
     </row>
-    <row r="8" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="32" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="J8" s="28"/>
       <c r="L8" s="22" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N8" s="23" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="O8" s="22" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="P8" s="22" t="n">
         <v>8</v>
       </c>
       <c r="Q8" s="22" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="R8" s="23"/>
       <c r="S8" s="34" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="T8" s="22" t="n">
         <v>5</v>
       </c>
       <c r="U8" s="29" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="V8" s="29"/>
       <c r="W8" s="29" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="X8" s="29" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="Y8" s="29"/>
       <c r="Z8" s="29"/>
       <c r="AA8" s="29" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="AB8" s="30"/>
       <c r="AC8" s="24"/>
       <c r="AD8" s="25"/>
       <c r="AE8" s="26" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="AF8" s="25"/>
       <c r="AG8" s="27"/>
       <c r="AL8" s="22" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="AU8" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="AX8" s="23"/>
-      <c r="BE8" s="27"/>
-      <c r="BF8" s="27"/>
-      <c r="BG8" s="28"/>
-      <c r="BH8" s="28"/>
-      <c r="BI8" s="28"/>
+        <v>190</v>
+      </c>
+      <c r="BA8" s="23"/>
+      <c r="BH8" s="27"/>
+      <c r="BI8" s="27"/>
       <c r="BJ8" s="28"/>
       <c r="BK8" s="28"/>
-      <c r="AMA8" s="28"/>
-      <c r="AMB8" s="28"/>
-      <c r="AMC8" s="28"/>
+      <c r="BL8" s="28"/>
+      <c r="BM8" s="28"/>
+      <c r="BN8" s="28"/>
       <c r="AMD8" s="28"/>
       <c r="AME8" s="28"/>
       <c r="AMF8" s="28"/>
@@ -2314,69 +2320,66 @@
       <c r="AMI8" s="28"/>
       <c r="AMJ8" s="28"/>
     </row>
-    <row r="9" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="32" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="N9" s="23" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="O9" s="22" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="P9" s="22" t="n">
         <v>12</v>
       </c>
       <c r="Q9" s="23" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="R9" s="23"/>
       <c r="T9" s="22" t="n">
         <v>17</v>
       </c>
       <c r="U9" s="22" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="AA9" s="22" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="AB9" s="30"/>
       <c r="AC9" s="24"/>
       <c r="AD9" s="25"/>
       <c r="AE9" s="26" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="AF9" s="25"/>
       <c r="AG9" s="27"/>
-      <c r="AX9" s="23"/>
-      <c r="BE9" s="27"/>
-      <c r="BF9" s="27"/>
-      <c r="BG9" s="28"/>
-      <c r="BH9" s="28"/>
-      <c r="BI9" s="28"/>
+      <c r="BA9" s="23"/>
+      <c r="BH9" s="27"/>
+      <c r="BI9" s="27"/>
       <c r="BJ9" s="28"/>
       <c r="BK9" s="28"/>
-      <c r="AMA9" s="28"/>
-      <c r="AMB9" s="28"/>
-      <c r="AMC9" s="28"/>
+      <c r="BL9" s="28"/>
+      <c r="BM9" s="28"/>
+      <c r="BN9" s="28"/>
       <c r="AMD9" s="28"/>
       <c r="AME9" s="28"/>
       <c r="AMF9" s="28"/>
@@ -2385,26 +2388,26 @@
       <c r="AMI9" s="28"/>
       <c r="AMJ9" s="28"/>
     </row>
-    <row r="10" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="32" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D10" s="28"/>
       <c r="E10" s="22" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="G10" s="28"/>
       <c r="L10" s="22" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="N10" s="29" t="n">
         <v>20200130</v>
@@ -2413,40 +2416,37 @@
         <v>3</v>
       </c>
       <c r="P10" s="29" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="Q10" s="29" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="R10" s="23"/>
       <c r="T10" s="22" t="n">
         <v>17</v>
       </c>
       <c r="U10" s="22" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="AA10" s="22" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="AB10" s="30"/>
       <c r="AC10" s="26"/>
       <c r="AD10" s="25"/>
       <c r="AE10" s="26" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AF10" s="25"/>
       <c r="AG10" s="27"/>
-      <c r="AX10" s="23"/>
-      <c r="BE10" s="27"/>
-      <c r="BF10" s="27"/>
-      <c r="BG10" s="28"/>
-      <c r="BH10" s="28"/>
-      <c r="BI10" s="28"/>
+      <c r="BA10" s="23"/>
+      <c r="BH10" s="27"/>
+      <c r="BI10" s="27"/>
       <c r="BJ10" s="28"/>
       <c r="BK10" s="28"/>
-      <c r="AMA10" s="28"/>
-      <c r="AMB10" s="28"/>
-      <c r="AMC10" s="28"/>
+      <c r="BL10" s="28"/>
+      <c r="BM10" s="28"/>
+      <c r="BN10" s="28"/>
       <c r="AMD10" s="28"/>
       <c r="AME10" s="28"/>
       <c r="AMF10" s="28"/>
@@ -2457,16 +2457,16 @@
     </row>
     <row r="11" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="35" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="L11" s="28"/>
       <c r="N11" s="28"/>
@@ -2479,20 +2479,17 @@
       <c r="AC11" s="26"/>
       <c r="AD11" s="25"/>
       <c r="AE11" s="37" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="AF11" s="25"/>
       <c r="AG11" s="27"/>
-      <c r="BE11" s="27"/>
-      <c r="BF11" s="27"/>
-      <c r="BG11" s="28"/>
-      <c r="BH11" s="28"/>
-      <c r="BI11" s="28"/>
+      <c r="BH11" s="27"/>
+      <c r="BI11" s="27"/>
       <c r="BJ11" s="28"/>
       <c r="BK11" s="28"/>
-      <c r="AMA11" s="28"/>
-      <c r="AMB11" s="28"/>
-      <c r="AMC11" s="28"/>
+      <c r="BL11" s="28"/>
+      <c r="BM11" s="28"/>
+      <c r="BN11" s="28"/>
       <c r="AMD11" s="28"/>
       <c r="AME11" s="28"/>
       <c r="AMF11" s="28"/>
@@ -2501,21 +2498,21 @@
       <c r="AMI11" s="28"/>
       <c r="AMJ11" s="28"/>
     </row>
-    <row r="12" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="38" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="N12" s="28"/>
       <c r="O12" s="28"/>
@@ -2529,16 +2526,13 @@
       <c r="AE12" s="26"/>
       <c r="AF12" s="25"/>
       <c r="AG12" s="27"/>
-      <c r="BE12" s="27"/>
-      <c r="BF12" s="27"/>
-      <c r="BG12" s="28"/>
-      <c r="BH12" s="28"/>
-      <c r="BI12" s="28"/>
+      <c r="BH12" s="27"/>
+      <c r="BI12" s="27"/>
       <c r="BJ12" s="28"/>
       <c r="BK12" s="28"/>
-      <c r="AMA12" s="28"/>
-      <c r="AMB12" s="28"/>
-      <c r="AMC12" s="28"/>
+      <c r="BL12" s="28"/>
+      <c r="BM12" s="28"/>
+      <c r="BN12" s="28"/>
       <c r="AMD12" s="28"/>
       <c r="AME12" s="28"/>
       <c r="AMF12" s="28"/>
@@ -2547,18 +2541,18 @@
       <c r="AMI12" s="28"/>
       <c r="AMJ12" s="28"/>
     </row>
-    <row r="13" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="39" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G13" s="14"/>
       <c r="J13" s="28"/>
@@ -2574,16 +2568,13 @@
       <c r="AE13" s="26"/>
       <c r="AF13" s="25"/>
       <c r="AG13" s="27"/>
-      <c r="BE13" s="27"/>
-      <c r="BF13" s="27"/>
-      <c r="BG13" s="28"/>
-      <c r="BH13" s="28"/>
-      <c r="BI13" s="28"/>
+      <c r="BH13" s="27"/>
+      <c r="BI13" s="27"/>
       <c r="BJ13" s="28"/>
       <c r="BK13" s="28"/>
-      <c r="AMA13" s="28"/>
-      <c r="AMB13" s="28"/>
-      <c r="AMC13" s="28"/>
+      <c r="BL13" s="28"/>
+      <c r="BM13" s="28"/>
+      <c r="BN13" s="28"/>
       <c r="AMD13" s="28"/>
       <c r="AME13" s="28"/>
       <c r="AMF13" s="28"/>
@@ -2592,18 +2583,18 @@
       <c r="AMI13" s="28"/>
       <c r="AMJ13" s="28"/>
     </row>
-    <row r="14" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="39" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="G14" s="14"/>
       <c r="N14" s="28"/>
@@ -2618,16 +2609,13 @@
       <c r="AE14" s="26"/>
       <c r="AF14" s="25"/>
       <c r="AG14" s="27"/>
-      <c r="BE14" s="27"/>
-      <c r="BF14" s="27"/>
-      <c r="BG14" s="28"/>
-      <c r="BH14" s="28"/>
-      <c r="BI14" s="28"/>
+      <c r="BH14" s="27"/>
+      <c r="BI14" s="27"/>
       <c r="BJ14" s="28"/>
       <c r="BK14" s="28"/>
-      <c r="AMA14" s="28"/>
-      <c r="AMB14" s="28"/>
-      <c r="AMC14" s="28"/>
+      <c r="BL14" s="28"/>
+      <c r="BM14" s="28"/>
+      <c r="BN14" s="28"/>
       <c r="AMD14" s="28"/>
       <c r="AME14" s="28"/>
       <c r="AMF14" s="28"/>
@@ -2636,15 +2624,15 @@
       <c r="AMI14" s="28"/>
       <c r="AMJ14" s="28"/>
     </row>
-    <row r="15" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="39" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="N15" s="28"/>
       <c r="O15" s="28"/>
@@ -2658,16 +2646,13 @@
       <c r="AE15" s="26"/>
       <c r="AF15" s="25"/>
       <c r="AG15" s="27"/>
-      <c r="BE15" s="27"/>
-      <c r="BF15" s="27"/>
-      <c r="BG15" s="28"/>
-      <c r="BH15" s="28"/>
-      <c r="BI15" s="28"/>
+      <c r="BH15" s="27"/>
+      <c r="BI15" s="27"/>
       <c r="BJ15" s="28"/>
       <c r="BK15" s="28"/>
-      <c r="AMA15" s="28"/>
-      <c r="AMB15" s="28"/>
-      <c r="AMC15" s="28"/>
+      <c r="BL15" s="28"/>
+      <c r="BM15" s="28"/>
+      <c r="BN15" s="28"/>
       <c r="AMD15" s="28"/>
       <c r="AME15" s="28"/>
       <c r="AMF15" s="28"/>
@@ -2676,26 +2661,25 @@
       <c r="AMI15" s="28"/>
       <c r="AMJ15" s="28"/>
     </row>
-    <row r="16" s="42" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="42" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="40" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
-    <row r="17" s="42" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="42" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="43" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="44" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
@@ -2734,10 +2718,9 @@
       <c r="J21" s="44"/>
       <c r="K21" s="44"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="45" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B23" s="46"/>
       <c r="C23" s="46"/>
@@ -2796,7 +2779,10 @@
       <c r="BD23" s="46"/>
       <c r="BE23" s="46"/>
       <c r="BF23" s="46"/>
-      <c r="BG23" s="47"/>
+      <c r="BG23" s="46"/>
+      <c r="BH23" s="46"/>
+      <c r="BI23" s="46"/>
+      <c r="BJ23" s="47"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="48"/>
@@ -2857,7 +2843,10 @@
       <c r="BD24" s="49"/>
       <c r="BE24" s="49"/>
       <c r="BF24" s="49"/>
-      <c r="BG24" s="50"/>
+      <c r="BG24" s="49"/>
+      <c r="BH24" s="49"/>
+      <c r="BI24" s="49"/>
+      <c r="BJ24" s="50"/>
     </row>
     <row r="25" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="51"/>
@@ -2918,7 +2907,10 @@
       <c r="BD25" s="52"/>
       <c r="BE25" s="52"/>
       <c r="BF25" s="52"/>
-      <c r="BG25" s="53"/>
+      <c r="BG25" s="52"/>
+      <c r="BH25" s="52"/>
+      <c r="BI25" s="52"/>
+      <c r="BJ25" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2929,7 +2921,7 @@
     <mergeCell ref="X4:X6"/>
     <mergeCell ref="AT4:AT6"/>
     <mergeCell ref="AV4:AV6"/>
-    <mergeCell ref="AX4:AX6"/>
+    <mergeCell ref="BA4:BA6"/>
     <mergeCell ref="G12:G14"/>
     <mergeCell ref="A19:K21"/>
   </mergeCells>

</xml_diff>

<commit_message>
rename sample_name to sample_name_gpcf
</commit_message>
<xml_diff>
--- a/sequencing_spreadsheet.template.xlsx
+++ b/sequencing_spreadsheet.template.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">PATIENT_ID</t>
   </si>
   <si>
-    <t xml:space="preserve">SAMPLE_ID</t>
+    <t xml:space="preserve">SAMPLE_NAME_GPCF</t>
   </si>
   <si>
     <t xml:space="preserve">examples for organ shortcuts, always small</t>
@@ -1290,8 +1290,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AQ1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AZ2" activeCellId="0" sqref="AZ2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BF8" activeCellId="0" sqref="BF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>